<commit_message>
Get_Hotels REFramework integration and testing/debugging
</commit_message>
<xml_diff>
--- a/P2_Performer/Data/Config.xlsx
+++ b/P2_Performer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\GetawayGurus\P2_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB80386-3CDC-4A20-B2C8-464B672C67BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADF2BE5-D45E-4F48-9A31-5014831CCBED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2820" windowWidth="17300" windowHeight="9980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -171,14 +171,23 @@
     <t>Key for the weather api</t>
   </si>
   <si>
-    <t>ccs_test</t>
+    <t>activitiesKey</t>
+  </si>
+  <si>
+    <t>ActivitiesAPIKey</t>
+  </si>
+  <si>
+    <t>Key for the foursquare api</t>
+  </si>
+  <si>
+    <t>tripQueue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -202,6 +211,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF464E55"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -223,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -233,6 +249,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,19 +566,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18.5">
+    <row r="1" spans="1:26" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -600,13 +617,13 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
@@ -620,7 +637,7 @@
     <row r="4" spans="1:26">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:26" ht="29">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -646,15 +663,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18.5">
+    <row r="1" spans="1:26" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -688,7 +705,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -699,7 +716,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -812,7 +829,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -833,16 +850,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="30.1796875" customWidth="1"/>
-    <col min="3" max="3" width="60.26953125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.77734375" customWidth="1"/>
+    <col min="2" max="2" width="30.21875" customWidth="1"/>
+    <col min="3" max="3" width="60.21875" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -895,7 +912,20 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1896,5 +1926,6 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>